<commit_message>
added dh to monday q3 education
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@1727 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/Agendas/201309 WGM FHIR Agenda.xlsx
+++ b/documents/Agendas/201309 WGM FHIR Agenda.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="2550" windowWidth="19785" windowHeight="10875"/>
+    <workbookView xWindow="-640" yWindow="-18440" windowWidth="27840" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="76">
   <si>
     <t>Clinical Genomics</t>
   </si>
@@ -240,6 +244,9 @@
   </si>
   <si>
     <t>w/EHR</t>
+  </si>
+  <si>
+    <t>DH</t>
   </si>
 </sst>
 </file>
@@ -354,7 +361,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -364,7 +371,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -741,33 +748,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="4.42578125" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" style="9" customWidth="1"/>
-    <col min="11" max="13" width="4.42578125" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" style="9" customWidth="1"/>
-    <col min="15" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="4.42578125" style="9" customWidth="1"/>
-    <col min="19" max="21" width="4.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="4.42578125" style="9" customWidth="1"/>
-    <col min="23" max="23" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="4.5" customWidth="1"/>
+    <col min="10" max="10" width="4.5" style="9" customWidth="1"/>
+    <col min="11" max="13" width="4.5" customWidth="1"/>
+    <col min="14" max="14" width="4.5" style="9" customWidth="1"/>
+    <col min="15" max="17" width="4.5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5" style="9" customWidth="1"/>
+    <col min="19" max="21" width="4.5" style="1" customWidth="1"/>
+    <col min="22" max="22" width="4.5" style="9" customWidth="1"/>
+    <col min="23" max="23" width="4.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1">
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="10"/>
@@ -801,7 +808,7 @@
       </c>
       <c r="W1" s="32"/>
     </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="1" customFormat="1">
       <c r="A2" s="6" t="s">
         <v>61</v>
       </c>
@@ -872,7 +879,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="1" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
@@ -900,7 +907,7 @@
       </c>
       <c r="W3" s="5"/>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="1" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -930,7 +937,7 @@
       </c>
       <c r="W4" s="5"/>
     </row>
-    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="1" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -957,7 +964,7 @@
       <c r="V5" s="16"/>
       <c r="W5" s="5"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -985,7 +992,7 @@
       <c r="V6" s="16"/>
       <c r="W6" s="5"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -1013,7 +1020,7 @@
       <c r="V7" s="16"/>
       <c r="W7" s="5"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1039,7 +1046,7 @@
       <c r="V8" s="16"/>
       <c r="W8" s="5"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1055,7 +1062,9 @@
       <c r="E9" s="11"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
       <c r="N9" s="8"/>
@@ -1063,7 +1072,7 @@
       <c r="V9" s="16"/>
       <c r="W9" s="5"/>
     </row>
-    <row r="10" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" s="1" customFormat="1">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
@@ -1091,7 +1100,7 @@
       <c r="V10" s="16"/>
       <c r="W10" s="5"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1113,7 +1122,7 @@
       <c r="V11" s="16"/>
       <c r="W11" s="5"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1146,7 +1155,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1174,7 +1183,7 @@
       <c r="V13" s="16"/>
       <c r="W13" s="5"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -1201,7 +1210,7 @@
       <c r="V14" s="16"/>
       <c r="W14" s="5"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -1225,7 +1234,7 @@
       <c r="V15" s="16"/>
       <c r="W15" s="5"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -1255,7 +1264,7 @@
       <c r="V16" s="16"/>
       <c r="W16" s="5"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1287,7 +1296,7 @@
       <c r="V17" s="16"/>
       <c r="W17" s="5"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
@@ -1317,7 +1326,7 @@
       <c r="V18" s="16"/>
       <c r="W18" s="5"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
@@ -1346,7 +1355,7 @@
       <c r="V19" s="16"/>
       <c r="W19" s="5"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1381,7 +1390,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -1411,7 +1420,7 @@
       <c r="V21" s="16"/>
       <c r="W21" s="5"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
@@ -1438,7 +1447,7 @@
       <c r="V22" s="16"/>
       <c r="W22" s="5"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
@@ -1466,7 +1475,7 @@
       <c r="V23" s="16"/>
       <c r="W23" s="5"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23">
       <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
@@ -1493,7 +1502,7 @@
       <c r="V24" s="16"/>
       <c r="W24" s="5"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23">
       <c r="A25" s="29" t="s">
         <v>25</v>
       </c>
@@ -1520,7 +1529,7 @@
       <c r="V25" s="16"/>
       <c r="W25" s="5"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
@@ -1542,7 +1551,7 @@
       <c r="V26" s="16"/>
       <c r="W26" s="5"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
@@ -1564,7 +1573,7 @@
       <c r="V27" s="16"/>
       <c r="W27" s="5"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23">
       <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
@@ -1592,7 +1601,7 @@
       <c r="V28" s="16"/>
       <c r="W28" s="5"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -1620,7 +1629,7 @@
       <c r="V29" s="16"/>
       <c r="W29" s="5"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23">
       <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
@@ -1647,7 +1656,7 @@
       <c r="V30" s="16"/>
       <c r="W30" s="5"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23">
       <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
@@ -1673,7 +1682,7 @@
       <c r="V31" s="16"/>
       <c r="W31" s="5"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23">
       <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
@@ -1698,7 +1707,7 @@
       <c r="V32" s="16"/>
       <c r="W32" s="5"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23">
       <c r="A33" s="3" t="s">
         <v>33</v>
       </c>
@@ -1727,7 +1736,7 @@
       <c r="V33" s="16"/>
       <c r="W33" s="5"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23">
       <c r="K35">
         <v>3</v>
       </c>
@@ -1756,7 +1765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23">
       <c r="E41" s="14" t="s">
         <v>71</v>
       </c>
@@ -1770,6 +1779,11 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added dh to spa q1
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@1739 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/Agendas/201309 WGM FHIR Agenda.xlsx
+++ b/documents/Agendas/201309 WGM FHIR Agenda.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-640" yWindow="-18440" windowWidth="27840" windowHeight="18000"/>
+    <workbookView xWindow="-260" yWindow="-18360" windowWidth="27840" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="76">
   <si>
     <t>Clinical Genomics</t>
   </si>
@@ -755,7 +755,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1622,6 +1622,9 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="8"/>
+      <c r="K29" t="s">
+        <v>75</v>
+      </c>
       <c r="N29" s="23" t="s">
         <v>74</v>
       </c>

</xml_diff>